<commit_message>
finished aggregation but need to rerun acs_data before aggregating to correct 2006 mistake
</commit_message>
<xml_diff>
--- a/acs/statistics.xlsx
+++ b/acs/statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Downloads\RA Work\acs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kguan17/Documents/GitHub/RA-Work/acs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFADA02A-7F34-4B71-97F3-2685682C0606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2322E60A-68B8-A04C-9CF5-B8F40AD74E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21555" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="1960" windowWidth="21560" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,15 +251,6 @@
     <t>DP03_0008E-DP03_0011E</t>
   </si>
   <si>
-    <t>DP05_0003E/100</t>
-  </si>
-  <si>
-    <t>DP05_0027E/100</t>
-  </si>
-  <si>
-    <t>DP05_0031E/100</t>
-  </si>
-  <si>
     <t>DP03_0119PE</t>
   </si>
   <si>
@@ -267,6 +258,15 @@
   </si>
   <si>
     <t>DP03_0121PE</t>
+  </si>
+  <si>
+    <t>DP05_0027E</t>
+  </si>
+  <si>
+    <t>DP05_0031E</t>
+  </si>
+  <si>
+    <t>DP05_0003E</t>
   </si>
 </sst>
 </file>
@@ -601,17 +601,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -622,9 +622,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -633,9 +633,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -644,15 +644,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -663,7 +663,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -674,7 +674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -682,7 +682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -693,7 +693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -704,7 +704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -712,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -723,7 +723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -734,7 +734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -745,7 +745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -753,7 +753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -761,7 +761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -772,7 +772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -783,7 +783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -794,7 +794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -805,7 +805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -816,7 +816,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -827,7 +827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -838,7 +838,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -849,7 +849,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -860,7 +860,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>39</v>
       </c>
@@ -871,7 +871,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
@@ -882,7 +882,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
@@ -893,7 +893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -904,7 +904,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -915,7 +915,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -926,7 +926,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -937,7 +937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -948,7 +948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -959,7 +959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
@@ -970,7 +970,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -981,7 +981,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
@@ -992,7 +992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>54</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
@@ -1022,10 +1022,10 @@
         <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>57</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>58</v>
       </c>
@@ -1044,10 +1044,10 @@
         <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>